<commit_message>
cambios seguir pared 19-oct
</commit_message>
<xml_diff>
--- a/Firmware/Examples/turnMaze/simulacionGiro.xlsx
+++ b/Firmware/Examples/turnMaze/simulacionGiro.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>accW</t>
   </si>
@@ -319,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -340,6 +340,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,79 +456,79 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.098878736696445</c:v>
+                  <c:v>2.647482478011952</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.197757473392889</c:v>
+                  <c:v>5.294964956023904</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.296636210089334</c:v>
+                  <c:v>7.942447434035854</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.395514946785778</c:v>
+                  <c:v>10.58992991204781</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.49439368348222</c:v>
+                  <c:v>13.23741239005976</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.59327242017867</c:v>
+                  <c:v>15.88489486807171</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.69215115687511</c:v>
+                  <c:v>18.53237734608366</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16.79102989357156</c:v>
+                  <c:v>21.17985982409561</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18.76800865066574</c:v>
+                  <c:v>23.70544232250531</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19.86688738736219</c:v>
+                  <c:v>25.35292480051725</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>20.96576612405863</c:v>
+                  <c:v>27.00040727852921</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>22.06464486075508</c:v>
+                  <c:v>25.71903201785324</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>23.16352359745152</c:v>
+                  <c:v>24.43765675717728</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>21.88214833677556</c:v>
+                  <c:v>23.15628149650132</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>20.6007730760996</c:v>
+                  <c:v>21.87490623582536</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>19.31939781542364</c:v>
+                  <c:v>20.5935309751494</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17.03802255474768</c:v>
+                  <c:v>18.31215571447344</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>14.75664729407172</c:v>
+                  <c:v>16.03078045379748</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>12.47527203339575</c:v>
+                  <c:v>13.74940519312151</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>10.19389677271979</c:v>
+                  <c:v>11.46802993244555</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.912521512043827</c:v>
+                  <c:v>9.186654671769588</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5.631146251367865</c:v>
+                  <c:v>6.905279411093626</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.349770990691903</c:v>
+                  <c:v>4.623904150417664</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.068395730015941</c:v>
+                  <c:v>2.342528889741702</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.0</c:v>
+                  <c:v>0.183053608668001</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>0.0</c:v>
@@ -700,79 +701,79 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0988787366964447</c:v>
+                  <c:v>0.647482478011952</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.197757473392889</c:v>
+                  <c:v>1.294964956023903</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.296636210089334</c:v>
+                  <c:v>1.942447434035855</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.395514946785779</c:v>
+                  <c:v>2.589929912047807</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.494393683482224</c:v>
+                  <c:v>3.237412390059758</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.593272420178669</c:v>
+                  <c:v>3.88489486807171</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.692151156875115</c:v>
+                  <c:v>4.532377346083661</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.79102989357156</c:v>
+                  <c:v>5.179859824095614</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.011808609870267</c:v>
+                  <c:v>5.949242281709826</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.110687346566712</c:v>
+                  <c:v>7.596724759721777</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.209566083263157</c:v>
+                  <c:v>9.244207237733729</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.308444819959602</c:v>
+                  <c:v>7.962831977057768</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.407323556656047</c:v>
+                  <c:v>6.681456716381806</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.125948295980084</c:v>
+                  <c:v>5.400081455705844</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.844573035304123</c:v>
+                  <c:v>4.118706195029883</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.563197774628161</c:v>
+                  <c:v>2.837330934353922</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.2818225139522</c:v>
+                  <c:v>2.55595567367796</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.000447253276238</c:v>
+                  <c:v>2.274580413002</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.719071992600275</c:v>
+                  <c:v>1.993205152326037</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.437696731924313</c:v>
+                  <c:v>1.711829891650074</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.156321471248351</c:v>
+                  <c:v>1.430454630974112</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-0.125053789427612</c:v>
+                  <c:v>1.14907937029815</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-0.406429050103574</c:v>
+                  <c:v>0.867704109622188</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-0.687804310779536</c:v>
+                  <c:v>0.586328848946225</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.0</c:v>
+                  <c:v>0.183053608668001</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>0.0</c:v>
@@ -1924,79 +1925,79 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.098878736696445</c:v>
+                  <c:v>1.647482478011952</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.197757473392889</c:v>
+                  <c:v>3.294964956023903</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.296636210089334</c:v>
+                  <c:v>4.942447434035854</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.395514946785779</c:v>
+                  <c:v>6.589929912047806</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.494393683482224</c:v>
+                  <c:v>8.237412390059758</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.59327242017867</c:v>
+                  <c:v>9.88489486807171</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.692151156875115</c:v>
+                  <c:v>11.53237734608366</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.79102989357156</c:v>
+                  <c:v>13.17985982409561</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.889908630268004</c:v>
+                  <c:v>14.82734230210757</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.98878736696445</c:v>
+                  <c:v>16.47482478011952</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12.0876661036609</c:v>
+                  <c:v>18.12230725813147</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13.18654484035734</c:v>
+                  <c:v>16.84093199745551</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14.28542357705379</c:v>
+                  <c:v>15.55955673677954</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>13.00404831637782</c:v>
+                  <c:v>14.27818147610358</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11.72267305570186</c:v>
+                  <c:v>12.99680621542762</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10.4412977950259</c:v>
+                  <c:v>11.71543095475166</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9.159922534349938</c:v>
+                  <c:v>10.4340556940757</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.878547273673976</c:v>
+                  <c:v>9.152680433399737</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.597172012998014</c:v>
+                  <c:v>7.871305172723775</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.315796752322051</c:v>
+                  <c:v>6.589929912047813</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.03442149164609</c:v>
+                  <c:v>5.308554651371851</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.753046230970127</c:v>
+                  <c:v>4.027179390695888</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.471670970294165</c:v>
+                  <c:v>2.745804130019926</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.190295709618202</c:v>
+                  <c:v>1.464428869343964</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.0</c:v>
+                  <c:v>0.183053608668001</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>0.0</c:v>
@@ -2449,217 +2450,217 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.098878736696445</c:v>
+                  <c:v>2.647482478011952</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.296636210089334</c:v>
+                  <c:v>7.942447434035855</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.59327242017867</c:v>
+                  <c:v>15.88489486807171</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.98878736696444</c:v>
+                  <c:v>26.47482478011952</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31.48318105044667</c:v>
+                  <c:v>39.71223717017927</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44.07645347062534</c:v>
+                  <c:v>55.597132038251</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>58.76860462750045</c:v>
+                  <c:v>74.12950938433465</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>75.559634521072</c:v>
+                  <c:v>95.30936920843027</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>94.32764317173774</c:v>
+                  <c:v>119.0148115309356</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>114.1945305590999</c:v>
+                  <c:v>144.3677363314528</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>135.1602966831586</c:v>
+                  <c:v>171.368143609982</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>157.2249415439136</c:v>
+                  <c:v>197.0871756278353</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>180.3884651413652</c:v>
+                  <c:v>221.5248323850125</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>202.2706134781407</c:v>
+                  <c:v>244.6811138815139</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>222.8713865542404</c:v>
+                  <c:v>266.5560201173392</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>242.190784369664</c:v>
+                  <c:v>287.1495510924886</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>259.2288069244117</c:v>
+                  <c:v>305.461706806962</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>273.9854542184834</c:v>
+                  <c:v>321.4924872607595</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>286.4607262518792</c:v>
+                  <c:v>335.241892453881</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>296.654623024599</c:v>
+                  <c:v>346.7099223863265</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>304.5671445366428</c:v>
+                  <c:v>355.8965770580962</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>310.1982907880106</c:v>
+                  <c:v>362.8018564691898</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>313.5480617787026</c:v>
+                  <c:v>367.4257606196074</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.7682895093491</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>314.6164575087185</c:v>
+                  <c:v>369.9513431180171</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2702,217 +2703,217 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0988787366964447</c:v>
+                  <c:v>0.647482478011952</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.296636210089334</c:v>
+                  <c:v>1.942447434035855</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.593272420178669</c:v>
+                  <c:v>3.88489486807171</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.988787366964448</c:v>
+                  <c:v>6.474824780119516</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.483181050446672</c:v>
+                  <c:v>9.712237170179275</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.076453470625341</c:v>
+                  <c:v>13.59713203825098</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.768604627500456</c:v>
+                  <c:v>18.12950938433465</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.559634521072016</c:v>
+                  <c:v>23.30936920843026</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.571443130942282</c:v>
+                  <c:v>29.25861149014009</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.682130477508994</c:v>
+                  <c:v>36.85533624986186</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.89169656077215</c:v>
+                  <c:v>46.0995434875956</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>14.20014138073175</c:v>
+                  <c:v>54.06237546465336</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>19.6074649373878</c:v>
+                  <c:v>60.74383218103517</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>23.73341323336788</c:v>
+                  <c:v>66.14391363674101</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>26.57798626867201</c:v>
+                  <c:v>70.2626198317709</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>28.14118404330017</c:v>
+                  <c:v>73.09995076612483</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>29.42300655725237</c:v>
+                  <c:v>75.65590643980279</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>30.42345381052861</c:v>
+                  <c:v>77.93048685280479</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>31.14252580312888</c:v>
+                  <c:v>79.92369200513083</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>31.5802225350532</c:v>
+                  <c:v>81.6355218967809</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>31.73654400630155</c:v>
+                  <c:v>83.06597652775501</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>31.61149021687394</c:v>
+                  <c:v>84.21505589805317</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>31.20506116677036</c:v>
+                  <c:v>85.08276000767535</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.66908885662157</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>30.51725685599083</c:v>
+                  <c:v>85.85214246528957</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3214,217 +3215,217 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.483405839437695</c:v>
+                  <c:v>0.72599094789519</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.67952700051911</c:v>
+                  <c:v>2.525004490439838</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.470777220036146</c:v>
+                  <c:v>5.219087367538243</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.849854290223527</c:v>
+                  <c:v>8.79718633056535</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.801144685872738</c:v>
+                  <c:v>13.23566778848646</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.296082036331</c:v>
+                  <c:v>18.4912932556847</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16.28764331895393</c:v>
+                  <c:v>24.49289172496712</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20.70421052151556</c:v>
+                  <c:v>31.1320758665935</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25.44658975113316</c:v>
+                  <c:v>38.25874398646804</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>30.41427832022504</c:v>
+                  <c:v>45.7208467546666</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>35.4948689636396</c:v>
+                  <c:v>53.34836357816952</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>40.56574130950631</c:v>
+                  <c:v>59.82883864387612</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>45.49593778026707</c:v>
+                  <c:v>65.19731817365687</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>49.42840299065193</c:v>
+                  <c:v>69.50848573374473</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>52.4388236431008</c:v>
+                  <c:v>72.83511917325264</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>54.61850427098542</c:v>
+                  <c:v>75.26629771572723</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>56.12475364889056</c:v>
+                  <c:v>76.96553479111774</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>57.10741932638228</c:v>
+                  <c:v>78.08986867762273</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>57.70257449605195</c:v>
+                  <c:v>78.78314938864198</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>58.02832377847511</c:v>
+                  <c:v>79.17155036435602</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>58.1822239312435</c:v>
+                  <c:v>79.36078692219296</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>58.23985013517028</c:v>
+                  <c:v>79.43455519579953</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>58.25410444361692</c:v>
+                  <c:v>79.45377023779568</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.4562658810424</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>58.25494670290161</c:v>
+                  <c:v>79.45657783644823</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3439,217 +3440,217 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.00658263439175403</c:v>
+                  <c:v>0.00993230848470453</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0460720680092146</c:v>
+                  <c:v>0.0695164820625665</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.164475858603428</c:v>
+                  <c:v>0.248171040709074</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.427255773218967</c:v>
+                  <c:v>0.644665442667485</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.918725809449417</c:v>
+                  <c:v>1.38620596596375</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.740796452739551</c:v>
+                  <c:v>2.626528887036044</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.010712909501279</c:v>
+                  <c:v>4.542466206863319</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.857379664203893</c:v>
+                  <c:v>7.328365331666071</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.409478898444938</c:v>
+                  <c:v>11.17811876651924</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.7454497412984</c:v>
+                  <c:v>16.20972112330814</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14.93037775101521</c:v>
+                  <c:v>22.52090065705457</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>20.01445117266</c:v>
+                  <c:v>29.05109536492929</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>26.03162405204549</c:v>
+                  <c:v>35.64119608785644</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>31.92059336148229</c:v>
+                  <c:v>42.14149102492246</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>37.54966016990448</c:v>
+                  <c:v>48.41393153553297</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>42.80099804716247</c:v>
+                  <c:v>54.33418245036852</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>47.5561057722222</c:v>
+                  <c:v>59.77500898331536</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>51.7322561979897</c:v>
+                  <c:v>64.64695657248919</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>55.27505595322614</c:v>
+                  <c:v>68.89070042146602</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>58.15134710301469</c:v>
+                  <c:v>72.46968696545643</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>60.34286478040765</c:v>
+                  <c:v>75.36350615904439</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>61.84090811899948</c:v>
+                  <c:v>77.56226904799106</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>62.64216906091108</c:v>
+                  <c:v>79.06214597032873</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.86214207767225</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>62.74578978248372</c:v>
+                  <c:v>79.96214159109018</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6472,8 +6473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="99" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="99" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6592,7 +6593,7 @@
       </c>
       <c r="P3">
         <f>2*PI()*C15/(C16)</f>
-        <v>0.5445427266222308</v>
+        <v>0.54628805587422513</v>
       </c>
       <c r="Q3">
         <f>(K3-L3)/$C$14</f>
@@ -6630,43 +6631,43 @@
       </c>
       <c r="I4">
         <f xml:space="preserve"> IF($F4 &lt; ($C$10 - $I3/$C$6*25), IF($I3+$C$5 &lt; $C$8, $I3+$C$5, $C$8), IF( $I3-$C$6 &gt; 0,$I3-$C$6, 0))</f>
-        <v>1.0988787366964448</v>
+        <v>1.6474824780119517</v>
       </c>
       <c r="J4">
         <f>I4+J3</f>
-        <v>1.0988787366964448</v>
+        <v>1.6474824780119517</v>
       </c>
       <c r="K4">
         <f t="shared" ref="K4:K67" si="0">I4+G4</f>
-        <v>2.0988787366964448</v>
+        <v>2.6474824780119519</v>
       </c>
       <c r="L4">
         <f t="shared" ref="L4:L67" si="1">I4-G4</f>
-        <v>9.8878736696444758E-2</v>
+        <v>0.64748247801195169</v>
       </c>
       <c r="M4">
         <f>K4+M3</f>
-        <v>2.0988787366964448</v>
+        <v>2.6474824780119519</v>
       </c>
       <c r="N4">
         <f>L4+N3</f>
-        <v>9.8878736696444758E-2</v>
+        <v>0.64748247801195169</v>
       </c>
       <c r="Q4">
         <f>360/(2*PI())*$P$3*(K4-L4)/$C$14</f>
-        <v>0.63030303030303025</v>
+        <v>0.63232323232323229</v>
       </c>
       <c r="R4">
         <f>Q4+R3</f>
-        <v>0.63030303030303025</v>
+        <v>0.63232323232323229</v>
       </c>
       <c r="S4">
         <f>S3+$P$3*((L4+K4)/2*COS(R4))</f>
-        <v>0.48340583943769511</v>
+        <v>0.72599094789519003</v>
       </c>
       <c r="T4">
         <f>T3+$P$3*((L4+K4)/2*SIN(RADIANS(R4)))</f>
-        <v>6.5826343917540333E-3</v>
+        <v>9.9323084847045291E-3</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.2">
@@ -6674,8 +6675,8 @@
         <v>4</v>
       </c>
       <c r="C5" s="6">
-        <f>120*D5*2/(2*3.14*15.65) /100</f>
-        <v>1.0988787366964448</v>
+        <f>180*D5*2/(2*PI()*15.65) /100</f>
+        <v>1.6474824780119517</v>
       </c>
       <c r="D5" s="7">
         <v>45</v>
@@ -6693,43 +6694,43 @@
       </c>
       <c r="I5">
         <f t="shared" ref="I5:I68" si="3" xml:space="preserve"> IF($F5 &lt; ($C$10 - $I4/$C$6*25), IF($I4+$C$5 &lt; $C$8, $I4+$C$5, $C$8), IF( $I4-$C$6 &gt; 0,$I4-$C$6, 0))</f>
-        <v>2.1977574733928895</v>
+        <v>3.2949649560239034</v>
       </c>
       <c r="J5">
         <f t="shared" ref="J5:J68" si="4">I5+J4</f>
-        <v>3.2966362100893343</v>
+        <v>4.9424474340358548</v>
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>4.1977574733928895</v>
+        <v>5.2949649560239038</v>
       </c>
       <c r="L5">
         <f t="shared" si="1"/>
-        <v>0.19775747339288952</v>
+        <v>1.2949649560239034</v>
       </c>
       <c r="M5">
         <f t="shared" ref="M5:M68" si="5">K5+M4</f>
-        <v>6.2966362100893338</v>
+        <v>7.9424474340358557</v>
       </c>
       <c r="N5">
         <f t="shared" ref="N5:N68" si="6">L5+N4</f>
-        <v>0.29663621008933427</v>
+        <v>1.9424474340358551</v>
       </c>
       <c r="Q5">
         <f t="shared" ref="Q5:Q68" si="7">360/(2*PI())*$P$3*(K5-L5)/$C$14</f>
-        <v>1.2606060606060605</v>
+        <v>1.2646464646464646</v>
       </c>
       <c r="R5">
         <f t="shared" ref="R5:R68" si="8">Q5+R4</f>
-        <v>1.8909090909090907</v>
+        <v>1.896969696969697</v>
       </c>
       <c r="S5">
         <f t="shared" ref="S5:S68" si="9">S4+$P$3*((L5+K5)/2*COS(RADIANS(R5)))</f>
-        <v>1.6795270005191103</v>
+        <v>2.5250044904398381</v>
       </c>
       <c r="T5">
         <f t="shared" ref="T5:T68" si="10">T4+$P$3*((L5+K5)/2*SIN(RADIANS(R5)))</f>
-        <v>4.607206800921463E-2</v>
+        <v>6.9516482062566498E-2</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.2">
@@ -6756,43 +6757,43 @@
       </c>
       <c r="I6">
         <f t="shared" si="3"/>
-        <v>3.2966362100893343</v>
+        <v>4.9424474340358548</v>
       </c>
       <c r="J6">
         <f t="shared" si="4"/>
-        <v>6.5932724201786685</v>
+        <v>9.8848948680717097</v>
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>6.2966362100893338</v>
+        <v>7.9424474340358548</v>
       </c>
       <c r="L6">
         <f t="shared" si="1"/>
-        <v>0.29663621008933427</v>
+        <v>1.9424474340358548</v>
       </c>
       <c r="M6">
         <f t="shared" si="5"/>
-        <v>12.593272420178668</v>
+        <v>15.884894868071711</v>
       </c>
       <c r="N6">
         <f t="shared" si="6"/>
-        <v>0.59327242017866855</v>
+        <v>3.8848948680717097</v>
       </c>
       <c r="Q6">
         <f t="shared" si="7"/>
-        <v>1.8909090909090909</v>
+        <v>1.8969696969696972</v>
       </c>
       <c r="R6">
         <f t="shared" si="8"/>
-        <v>3.7818181818181813</v>
+        <v>3.7939393939393939</v>
       </c>
       <c r="S6">
         <f t="shared" si="9"/>
-        <v>3.4707772200361457</v>
+        <v>5.2190873675382434</v>
       </c>
       <c r="T6">
         <f t="shared" si="10"/>
-        <v>0.16447585860342803</v>
+        <v>0.24817104070907423</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.2">
@@ -6819,43 +6820,43 @@
       </c>
       <c r="I7">
         <f t="shared" si="3"/>
-        <v>4.395514946785779</v>
+        <v>6.5899299120478068</v>
       </c>
       <c r="J7">
         <f t="shared" si="4"/>
-        <v>10.988787366964448</v>
+        <v>16.474824780119516</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>8.395514946785779</v>
+        <v>10.589929912047808</v>
       </c>
       <c r="L7">
         <f t="shared" si="1"/>
-        <v>0.39551494678577903</v>
+        <v>2.5899299120478068</v>
       </c>
       <c r="M7">
         <f t="shared" si="5"/>
-        <v>20.988787366964445</v>
+        <v>26.474824780119519</v>
       </c>
       <c r="N7">
         <f t="shared" si="6"/>
-        <v>0.98878736696444758</v>
+        <v>6.4748247801195165</v>
       </c>
       <c r="Q7">
         <f t="shared" si="7"/>
-        <v>2.521212121212121</v>
+        <v>2.5292929292929291</v>
       </c>
       <c r="R7">
         <f t="shared" si="8"/>
-        <v>6.3030303030303028</v>
+        <v>6.3232323232323235</v>
       </c>
       <c r="S7">
         <f>S6+$P$3*((L7+K7)/2*COS(RADIANS(R7)))</f>
-        <v>5.8498542902235275</v>
+        <v>8.7971863305653493</v>
       </c>
       <c r="T7">
         <f t="shared" si="10"/>
-        <v>0.42725577321896668</v>
+        <v>0.64466544266748549</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.2">
@@ -6882,43 +6883,43 @@
       </c>
       <c r="I8">
         <f t="shared" si="3"/>
-        <v>5.4943936834822242</v>
+        <v>8.2374123900597578</v>
       </c>
       <c r="J8">
         <f t="shared" si="4"/>
-        <v>16.483181050446674</v>
+        <v>24.712237170179272</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>10.494393683482224</v>
+        <v>13.237412390059758</v>
       </c>
       <c r="L8">
         <f t="shared" si="1"/>
-        <v>0.49439368348222423</v>
+        <v>3.2374123900597578</v>
       </c>
       <c r="M8">
         <f t="shared" si="5"/>
-        <v>31.483181050446667</v>
+        <v>39.712237170179279</v>
       </c>
       <c r="N8">
         <f t="shared" si="6"/>
-        <v>1.4831810504466718</v>
+        <v>9.7122371701792751</v>
       </c>
       <c r="Q8">
         <f t="shared" si="7"/>
-        <v>3.1515151515151514</v>
+        <v>3.1616161616161618</v>
       </c>
       <c r="R8">
         <f t="shared" si="8"/>
-        <v>9.4545454545454533</v>
+        <v>9.4848484848484844</v>
       </c>
       <c r="S8">
         <f t="shared" si="9"/>
-        <v>8.8011446858727389</v>
+        <v>13.23566778848646</v>
       </c>
       <c r="T8">
         <f t="shared" si="10"/>
-        <v>0.91872580944941717</v>
+        <v>1.3862059659637502</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.2">
@@ -6938,43 +6939,43 @@
       </c>
       <c r="I9">
         <f t="shared" si="3"/>
-        <v>6.5932724201786694</v>
+        <v>9.8848948680717097</v>
       </c>
       <c r="J9">
         <f t="shared" si="4"/>
-        <v>23.076453470625346</v>
+        <v>34.597132038250983</v>
       </c>
       <c r="K9">
         <f>I9+G9</f>
-        <v>12.593272420178669</v>
+        <v>15.88489486807171</v>
       </c>
       <c r="L9">
         <f>I9-G9</f>
-        <v>0.59327242017866944</v>
+        <v>3.8848948680717097</v>
       </c>
       <c r="M9">
         <f>K9+M8</f>
-        <v>44.076453470625339</v>
+        <v>55.59713203825099</v>
       </c>
       <c r="N9">
         <f t="shared" si="6"/>
-        <v>2.0764534706253412</v>
+        <v>13.597132038250985</v>
       </c>
       <c r="Q9">
         <f t="shared" si="7"/>
-        <v>3.7818181818181817</v>
+        <v>3.7939393939393944</v>
       </c>
       <c r="R9">
         <f t="shared" si="8"/>
-        <v>13.236363636363635</v>
+        <v>13.278787878787879</v>
       </c>
       <c r="S9">
         <f t="shared" si="9"/>
-        <v>12.296082036330995</v>
+        <v>18.491293255684695</v>
       </c>
       <c r="T9">
         <f t="shared" si="10"/>
-        <v>1.7407964527395512</v>
+        <v>2.6265288870360446</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.2">
@@ -6985,7 +6986,9 @@
         <f>_xlfn.FLOOR.MATH((C11+C12+C13)/25)*25</f>
         <v>625</v>
       </c>
-      <c r="D10" s="7"/>
+      <c r="D10" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="F10">
         <v>175</v>
       </c>
@@ -6999,43 +7002,43 @@
       </c>
       <c r="I10">
         <f t="shared" si="3"/>
-        <v>7.6921511568751146</v>
+        <v>11.532377346083662</v>
       </c>
       <c r="J10">
         <f t="shared" si="4"/>
-        <v>30.768604627500459</v>
+        <v>46.129509384334646</v>
       </c>
       <c r="K10">
         <f>I10+G10</f>
-        <v>14.692151156875115</v>
+        <v>18.532377346083663</v>
       </c>
       <c r="L10">
         <f>I10-G10</f>
-        <v>0.69215115687511464</v>
+        <v>4.5323773460836616</v>
       </c>
       <c r="M10">
         <f t="shared" si="5"/>
-        <v>58.768604627500451</v>
+        <v>74.129509384334654</v>
       </c>
       <c r="N10">
         <f t="shared" si="6"/>
-        <v>2.7686046275004559</v>
+        <v>18.129509384334646</v>
       </c>
       <c r="Q10">
         <f t="shared" si="7"/>
-        <v>4.4121212121212121</v>
+        <v>4.426262626262627</v>
       </c>
       <c r="R10">
         <f t="shared" si="8"/>
-        <v>17.648484848484848</v>
+        <v>17.705050505050508</v>
       </c>
       <c r="S10">
         <f t="shared" si="9"/>
-        <v>16.287643318953933</v>
+        <v>24.492891724967116</v>
       </c>
       <c r="T10">
         <f t="shared" si="10"/>
-        <v>3.0107129095012786</v>
+        <v>4.5424662068633195</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.2">
@@ -7062,43 +7065,43 @@
       </c>
       <c r="I11">
         <f t="shared" si="3"/>
-        <v>8.7910298935715598</v>
+        <v>13.179859824095614</v>
       </c>
       <c r="J11">
         <f t="shared" si="4"/>
-        <v>39.55963452107202</v>
+        <v>59.309369208430262</v>
       </c>
       <c r="K11">
         <f>I11+G11</f>
-        <v>16.791029893571562</v>
+        <v>21.179859824095615</v>
       </c>
       <c r="L11">
         <f>I11-G11</f>
-        <v>0.79102989357155984</v>
+        <v>5.1798598240956135</v>
       </c>
       <c r="M11">
         <f t="shared" si="5"/>
-        <v>75.559634521072013</v>
+        <v>95.309369208430269</v>
       </c>
       <c r="N11">
         <f t="shared" si="6"/>
-        <v>3.5596345210720157</v>
+        <v>23.309369208430262</v>
       </c>
       <c r="Q11">
         <f t="shared" si="7"/>
-        <v>5.042424242424242</v>
+        <v>5.0585858585858583</v>
       </c>
       <c r="R11">
         <f t="shared" si="8"/>
-        <v>22.690909090909091</v>
+        <v>22.763636363636365</v>
       </c>
       <c r="S11">
         <f t="shared" si="9"/>
-        <v>20.704210521515559</v>
+        <v>31.1320758665935</v>
       </c>
       <c r="T11">
         <f t="shared" si="10"/>
-        <v>4.8573796642038936</v>
+        <v>7.3283653316660713</v>
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.2">
@@ -7124,43 +7127,43 @@
       </c>
       <c r="I12">
         <f t="shared" si="3"/>
-        <v>9.889908630268005</v>
+        <v>14.827342302107565</v>
       </c>
       <c r="J12">
         <f t="shared" si="4"/>
-        <v>49.449543151340023</v>
+        <v>74.136711510537822</v>
       </c>
       <c r="K12">
         <f>I12+G12</f>
-        <v>18.768008650665742</v>
+        <v>23.705442322505306</v>
       </c>
       <c r="L12">
         <f>I12-G12</f>
-        <v>1.0118086098702666</v>
+        <v>5.9492422817098269</v>
       </c>
       <c r="M12">
         <f t="shared" si="5"/>
-        <v>94.327643171737748</v>
+        <v>119.01481153093557</v>
       </c>
       <c r="N12">
         <f t="shared" si="6"/>
-        <v>4.5714431309422823</v>
+        <v>29.25861149014009</v>
       </c>
       <c r="Q12">
         <f t="shared" si="7"/>
-        <v>5.5958933461900893</v>
+        <v>5.613828901786853</v>
       </c>
       <c r="R12">
         <f t="shared" si="8"/>
-        <v>28.28680243709918</v>
+        <v>28.377465265423218</v>
       </c>
       <c r="S12">
         <f t="shared" si="9"/>
-        <v>25.44658975113316</v>
+        <v>38.258743986468048</v>
       </c>
       <c r="T12">
         <f t="shared" si="10"/>
-        <v>7.4094788984449389</v>
+        <v>11.178118766519241</v>
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.2">
@@ -7187,43 +7190,43 @@
       </c>
       <c r="I13">
         <f t="shared" si="3"/>
-        <v>10.98878736696445</v>
+        <v>16.474824780119516</v>
       </c>
       <c r="J13">
         <f t="shared" si="4"/>
-        <v>60.438330518304475</v>
+        <v>90.611536290657341</v>
       </c>
       <c r="K13">
         <f>I13+G13</f>
-        <v>19.866887387362191</v>
+        <v>25.352924800517254</v>
       </c>
       <c r="L13">
         <f>I13-G13</f>
-        <v>2.1106873465667118</v>
+        <v>7.5967247597217771</v>
       </c>
       <c r="M13">
         <f t="shared" si="5"/>
-        <v>114.19453055909995</v>
+        <v>144.36773633145282</v>
       </c>
       <c r="N13">
         <f t="shared" si="6"/>
-        <v>6.682130477508994</v>
+        <v>36.855336249861864</v>
       </c>
       <c r="Q13">
         <f t="shared" si="7"/>
-        <v>5.5958933461900893</v>
+        <v>5.613828901786853</v>
       </c>
       <c r="R13">
         <f t="shared" si="8"/>
-        <v>33.882695783289272</v>
+        <v>33.991294167210071</v>
       </c>
       <c r="S13">
         <f t="shared" si="9"/>
-        <v>30.414278320225044</v>
+        <v>45.720846754666596</v>
       </c>
       <c r="T13">
         <f t="shared" si="10"/>
-        <v>10.745449741298396</v>
+        <v>16.209721123308135</v>
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.2">
@@ -7249,43 +7252,43 @@
       </c>
       <c r="I14">
         <f t="shared" si="3"/>
-        <v>12.087666103660895</v>
+        <v>18.122307258131467</v>
       </c>
       <c r="J14">
         <f t="shared" si="4"/>
-        <v>72.525996621965376</v>
+        <v>108.73384354878881</v>
       </c>
       <c r="K14">
         <f>I14+G14</f>
-        <v>20.965766124058632</v>
+        <v>27.000407278529206</v>
       </c>
       <c r="L14">
         <f>I14-G14</f>
-        <v>3.209566083263157</v>
+        <v>9.244207237733729</v>
       </c>
       <c r="M14">
         <f t="shared" si="5"/>
-        <v>135.16029668315858</v>
+        <v>171.36814360998201</v>
       </c>
       <c r="N14">
         <f t="shared" si="6"/>
-        <v>9.8916965607721501</v>
+        <v>46.099543487595597</v>
       </c>
       <c r="Q14">
         <f t="shared" si="7"/>
-        <v>5.5958933461900893</v>
+        <v>5.613828901786853</v>
       </c>
       <c r="R14">
         <f t="shared" si="8"/>
-        <v>39.47858912947936</v>
+        <v>39.605123068996924</v>
       </c>
       <c r="S14">
         <f t="shared" si="9"/>
-        <v>35.494868963639604</v>
+        <v>53.348363578169518</v>
       </c>
       <c r="T14">
         <f t="shared" si="10"/>
-        <v>14.930377751015214</v>
+        <v>22.520900657054568</v>
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.2">
@@ -7293,7 +7296,7 @@
         <v>28</v>
       </c>
       <c r="C15" s="16">
-        <v>15.6</v>
+        <v>15.65</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>29</v>
@@ -7311,43 +7314,43 @@
       </c>
       <c r="I15">
         <f t="shared" si="3"/>
-        <v>13.186544840357341</v>
+        <v>16.840931997455506</v>
       </c>
       <c r="J15">
         <f t="shared" si="4"/>
-        <v>85.712541462322719</v>
+        <v>125.57477554624433</v>
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
-        <v>22.064644860755081</v>
+        <v>25.719032017853245</v>
       </c>
       <c r="L15">
         <f t="shared" si="1"/>
-        <v>4.3084448199596022</v>
+        <v>7.9628319770577676</v>
       </c>
       <c r="M15">
         <f t="shared" si="5"/>
-        <v>157.22494154391364</v>
+        <v>197.08717562783525</v>
       </c>
       <c r="N15">
         <f t="shared" si="6"/>
-        <v>14.200141380731752</v>
+        <v>54.062375464653364</v>
       </c>
       <c r="Q15">
         <f t="shared" si="7"/>
-        <v>5.5958933461900893</v>
+        <v>5.613828901786853</v>
       </c>
       <c r="R15">
         <f t="shared" si="8"/>
-        <v>45.074482475669448</v>
+        <v>45.218951970783777</v>
       </c>
       <c r="S15">
         <f t="shared" si="9"/>
-        <v>40.565741309506308</v>
+        <v>59.828838643876118</v>
       </c>
       <c r="T15">
         <f t="shared" si="10"/>
-        <v>20.014451172659996</v>
+        <v>29.051095364929289</v>
       </c>
     </row>
     <row r="16" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -7374,43 +7377,43 @@
       </c>
       <c r="I16">
         <f t="shared" si="3"/>
-        <v>14.285423577053786</v>
+        <v>15.559556736779545</v>
       </c>
       <c r="J16">
         <f t="shared" si="4"/>
-        <v>99.99796503937651</v>
+        <v>141.13433228302387</v>
       </c>
       <c r="K16">
         <f t="shared" si="0"/>
-        <v>23.163523597451523</v>
+        <v>24.437656757177283</v>
       </c>
       <c r="L16">
         <f t="shared" si="1"/>
-        <v>5.4073235566560474</v>
+        <v>6.6814567163818062</v>
       </c>
       <c r="M16">
         <f t="shared" si="5"/>
-        <v>180.38846514136517</v>
+        <v>221.52483238501253</v>
       </c>
       <c r="N16">
         <f t="shared" si="6"/>
-        <v>19.6074649373878</v>
+        <v>60.743832181035174</v>
       </c>
       <c r="Q16">
         <f t="shared" si="7"/>
-        <v>5.5958933461900893</v>
+        <v>5.613828901786853</v>
       </c>
       <c r="R16">
         <f t="shared" si="8"/>
-        <v>50.670375821859537</v>
+        <v>50.83278087257063</v>
       </c>
       <c r="S16">
         <f t="shared" si="9"/>
-        <v>45.49593778026707</v>
+        <v>65.197318173656868</v>
       </c>
       <c r="T16">
         <f t="shared" si="10"/>
-        <v>26.031624052045487</v>
+        <v>35.641196087856443</v>
       </c>
     </row>
     <row r="17" spans="6:20" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -7427,43 +7430,43 @@
       </c>
       <c r="I17">
         <f t="shared" si="3"/>
-        <v>13.004048316377823</v>
+        <v>14.278181476103583</v>
       </c>
       <c r="J17">
         <f t="shared" si="4"/>
-        <v>113.00201335575433</v>
+        <v>155.41251375912745</v>
       </c>
       <c r="K17">
         <f t="shared" si="0"/>
-        <v>21.882148336775561</v>
+        <v>23.156281496501322</v>
       </c>
       <c r="L17">
         <f t="shared" si="1"/>
-        <v>4.1259482959800842</v>
+        <v>5.4000814557058447</v>
       </c>
       <c r="M17">
         <f t="shared" si="5"/>
-        <v>202.27061347814075</v>
+        <v>244.68111388151385</v>
       </c>
       <c r="N17">
         <f t="shared" si="6"/>
-        <v>23.733413233367884</v>
+        <v>66.143913636741019</v>
       </c>
       <c r="Q17">
         <f t="shared" si="7"/>
-        <v>5.5958933461900893</v>
+        <v>5.613828901786853</v>
       </c>
       <c r="R17">
         <f t="shared" si="8"/>
-        <v>56.266269168049625</v>
+        <v>56.446609774357484</v>
       </c>
       <c r="S17">
         <f t="shared" si="9"/>
-        <v>49.428402990651932</v>
+        <v>69.508485733744735</v>
       </c>
       <c r="T17">
         <f t="shared" si="10"/>
-        <v>31.92059336148229</v>
+        <v>42.141491024922459</v>
       </c>
     </row>
     <row r="18" spans="6:20" x14ac:dyDescent="0.2">
@@ -7480,43 +7483,43 @@
       </c>
       <c r="I18">
         <f t="shared" si="3"/>
-        <v>11.722673055701861</v>
+        <v>12.996806215427622</v>
       </c>
       <c r="J18">
         <f t="shared" si="4"/>
-        <v>124.72468641145619</v>
+        <v>168.40931997455507</v>
       </c>
       <c r="K18">
         <f>I18+G18</f>
-        <v>20.6007730760996</v>
+        <v>21.87490623582536</v>
       </c>
       <c r="L18">
         <f t="shared" si="1"/>
-        <v>2.8445730353041228</v>
+        <v>4.1187061950298833</v>
       </c>
       <c r="M18">
         <f t="shared" si="5"/>
-        <v>222.87138655424036</v>
+        <v>266.55602011733919</v>
       </c>
       <c r="N18">
         <f t="shared" si="6"/>
-        <v>26.577986268672007</v>
+        <v>70.262619831770905</v>
       </c>
       <c r="Q18">
         <f t="shared" si="7"/>
-        <v>5.5958933461900893</v>
+        <v>5.613828901786853</v>
       </c>
       <c r="R18">
         <f t="shared" si="8"/>
-        <v>61.862162514239714</v>
+        <v>62.060438676144337</v>
       </c>
       <c r="S18">
         <f t="shared" si="9"/>
-        <v>52.438823643100804</v>
+        <v>72.835119173252636</v>
       </c>
       <c r="T18">
         <f t="shared" si="10"/>
-        <v>37.549660169904477</v>
+        <v>48.413931535532974</v>
       </c>
     </row>
     <row r="19" spans="6:20" x14ac:dyDescent="0.2">
@@ -7533,43 +7536,43 @@
       </c>
       <c r="I19">
         <f t="shared" si="3"/>
-        <v>10.4412977950259</v>
+        <v>11.71543095475166</v>
       </c>
       <c r="J19">
         <f t="shared" si="4"/>
-        <v>135.16598420648208</v>
+        <v>180.12475092930674</v>
       </c>
       <c r="K19">
         <f t="shared" si="0"/>
-        <v>19.319397815423638</v>
+        <v>20.593530975149399</v>
       </c>
       <c r="L19">
         <f t="shared" si="1"/>
-        <v>1.5631977746281613</v>
+        <v>2.8373309343539219</v>
       </c>
       <c r="M19">
         <f t="shared" si="5"/>
-        <v>242.19078436966399</v>
+        <v>287.14955109248859</v>
       </c>
       <c r="N19">
         <f t="shared" si="6"/>
-        <v>28.141184043300168</v>
+        <v>73.099950766124834</v>
       </c>
       <c r="Q19">
         <f t="shared" si="7"/>
-        <v>5.5958933461900893</v>
+        <v>5.613828901786853</v>
       </c>
       <c r="R19">
         <f t="shared" si="8"/>
-        <v>67.458055860429809</v>
+        <v>67.67426757793119</v>
       </c>
       <c r="S19">
         <f t="shared" si="9"/>
-        <v>54.618504270985419</v>
+        <v>75.266297715727234</v>
       </c>
       <c r="T19">
         <f t="shared" si="10"/>
-        <v>42.800998047162466</v>
+        <v>54.334182450368523</v>
       </c>
     </row>
     <row r="20" spans="6:20" x14ac:dyDescent="0.2">
@@ -7586,43 +7589,43 @@
       </c>
       <c r="I20">
         <f t="shared" si="3"/>
-        <v>9.1599225343499384</v>
+        <v>10.434055694075699</v>
       </c>
       <c r="J20">
         <f t="shared" si="4"/>
-        <v>144.32590674083201</v>
+        <v>190.55880662338245</v>
       </c>
       <c r="K20">
         <f t="shared" si="0"/>
-        <v>17.038022554747677</v>
+        <v>18.312155714473437</v>
       </c>
       <c r="L20">
         <f t="shared" si="1"/>
-        <v>1.2818225139521999</v>
+        <v>2.5559556736779605</v>
       </c>
       <c r="M20">
         <f t="shared" si="5"/>
-        <v>259.22880692441169</v>
+        <v>305.46170680696201</v>
       </c>
       <c r="N20">
         <f t="shared" si="6"/>
-        <v>29.423006557252368</v>
+        <v>75.655906439802791</v>
       </c>
       <c r="Q20">
         <f t="shared" si="7"/>
-        <v>4.9655903158870593</v>
+        <v>4.9815056694636208</v>
       </c>
       <c r="R20">
         <f t="shared" si="8"/>
-        <v>72.423646176316865</v>
+        <v>72.655773247394805</v>
       </c>
       <c r="S20">
         <f t="shared" si="9"/>
-        <v>56.124753648890561</v>
+        <v>76.965534791117747</v>
       </c>
       <c r="T20">
         <f t="shared" si="10"/>
-        <v>47.556105772222196</v>
+        <v>59.77500898331536</v>
       </c>
     </row>
     <row r="21" spans="6:20" x14ac:dyDescent="0.2">
@@ -7639,43 +7642,43 @@
       </c>
       <c r="I21">
         <f t="shared" si="3"/>
-        <v>7.8785472736739761</v>
+        <v>9.1526804333997376</v>
       </c>
       <c r="J21">
         <f t="shared" si="4"/>
-        <v>152.20445401450598</v>
+        <v>199.71148705678218</v>
       </c>
       <c r="K21">
         <f t="shared" si="0"/>
-        <v>14.756647294071715</v>
+        <v>16.030780453797476</v>
       </c>
       <c r="L21">
         <f t="shared" si="1"/>
-        <v>1.0004472532762376</v>
+        <v>2.2745804130019991</v>
       </c>
       <c r="M21">
         <f t="shared" si="5"/>
-        <v>273.98545421848343</v>
+        <v>321.4924872607595</v>
       </c>
       <c r="N21">
         <f t="shared" si="6"/>
-        <v>30.423453810528606</v>
+        <v>77.93048685280479</v>
       </c>
       <c r="Q21">
         <f t="shared" si="7"/>
-        <v>4.3352872855840285</v>
+        <v>4.3491824371403878</v>
       </c>
       <c r="R21">
         <f t="shared" si="8"/>
-        <v>76.758933461900895</v>
+        <v>77.00495568453519</v>
       </c>
       <c r="S21">
         <f t="shared" si="9"/>
-        <v>57.107419326382278</v>
+        <v>78.089868677622732</v>
       </c>
       <c r="T21">
         <f t="shared" si="10"/>
-        <v>51.732256197989699</v>
+        <v>64.646956572489188</v>
       </c>
     </row>
     <row r="22" spans="6:20" x14ac:dyDescent="0.2">
@@ -7692,43 +7695,43 @@
       </c>
       <c r="I22">
         <f t="shared" si="3"/>
-        <v>6.5971720129980138</v>
+        <v>7.8713051727237753</v>
       </c>
       <c r="J22">
         <f t="shared" si="4"/>
-        <v>158.801626027504</v>
+        <v>207.58279222950594</v>
       </c>
       <c r="K22">
         <f t="shared" si="0"/>
-        <v>12.475272033395752</v>
+        <v>13.749405193121515</v>
       </c>
       <c r="L22">
         <f t="shared" si="1"/>
-        <v>0.71907199260027532</v>
+        <v>1.9932051523260368</v>
       </c>
       <c r="M22">
         <f t="shared" si="5"/>
-        <v>286.46072625187918</v>
+        <v>335.24189245388101</v>
       </c>
       <c r="N22">
         <f t="shared" si="6"/>
-        <v>31.142525803128883</v>
+        <v>79.923692005130832</v>
       </c>
       <c r="Q22">
         <f t="shared" si="7"/>
-        <v>3.7049842552809986</v>
+        <v>3.716859204817156</v>
       </c>
       <c r="R22">
         <f t="shared" si="8"/>
-        <v>80.4639177171819</v>
+        <v>80.721814889352345</v>
       </c>
       <c r="S22">
         <f t="shared" si="9"/>
-        <v>57.702574496051952</v>
+        <v>78.783149388641988</v>
       </c>
       <c r="T22">
         <f t="shared" si="10"/>
-        <v>55.275055953226143</v>
+        <v>68.890700421466022</v>
       </c>
     </row>
     <row r="23" spans="6:20" x14ac:dyDescent="0.2">
@@ -7745,43 +7748,43 @@
       </c>
       <c r="I23">
         <f t="shared" si="3"/>
-        <v>5.3157967523220515</v>
+        <v>6.589929912047813</v>
       </c>
       <c r="J23">
         <f t="shared" si="4"/>
-        <v>164.11742277982606</v>
+        <v>214.17272214155375</v>
       </c>
       <c r="K23">
         <f t="shared" si="0"/>
-        <v>10.193896772719789</v>
+        <v>11.468029932445551</v>
       </c>
       <c r="L23">
         <f t="shared" si="1"/>
-        <v>0.43769673192431302</v>
+        <v>1.7118298916500745</v>
       </c>
       <c r="M23">
         <f t="shared" si="5"/>
-        <v>296.65462302459895</v>
+        <v>346.70992238632658</v>
       </c>
       <c r="N23">
         <f t="shared" si="6"/>
-        <v>31.580222535053196</v>
+        <v>81.635521896780901</v>
       </c>
       <c r="Q23">
         <f t="shared" si="7"/>
-        <v>3.0746812249779683</v>
+        <v>3.0845359724939234</v>
       </c>
       <c r="R23">
         <f t="shared" si="8"/>
-        <v>83.538598942159865</v>
+        <v>83.806350861846269</v>
       </c>
       <c r="S23">
         <f t="shared" si="9"/>
-        <v>58.028323778475119</v>
+        <v>79.171550364356023</v>
       </c>
       <c r="T23">
         <f t="shared" si="10"/>
-        <v>58.151347103014693</v>
+        <v>72.469686965456432</v>
       </c>
     </row>
     <row r="24" spans="6:20" x14ac:dyDescent="0.2">
@@ -7798,43 +7801,43 @@
       </c>
       <c r="I24">
         <f t="shared" si="3"/>
-        <v>4.0344214916460892</v>
+        <v>5.3085546513718507</v>
       </c>
       <c r="J24">
         <f t="shared" si="4"/>
-        <v>168.15184427147216</v>
+        <v>219.4812767929256</v>
       </c>
       <c r="K24">
         <f t="shared" si="0"/>
-        <v>7.9125215120438277</v>
+        <v>9.1866546717695883</v>
       </c>
       <c r="L24">
         <f t="shared" si="1"/>
-        <v>0.15632147124835072</v>
+        <v>1.4304546309741122</v>
       </c>
       <c r="M24">
         <f t="shared" si="5"/>
-        <v>304.56714453664279</v>
+        <v>355.89657705809617</v>
       </c>
       <c r="N24">
         <f t="shared" si="6"/>
-        <v>31.736544006301546</v>
+        <v>83.065976527755012</v>
       </c>
       <c r="Q24">
         <f t="shared" si="7"/>
-        <v>2.4443781946749379</v>
+        <v>2.4522127401706912</v>
       </c>
       <c r="R24">
         <f t="shared" si="8"/>
-        <v>85.982977136834805</v>
+        <v>86.258563602016963</v>
       </c>
       <c r="S24">
         <f t="shared" si="9"/>
-        <v>58.182223931243499</v>
+        <v>79.360786922192958</v>
       </c>
       <c r="T24">
         <f t="shared" si="10"/>
-        <v>60.342864780407652</v>
+        <v>75.363506159044391</v>
       </c>
     </row>
     <row r="25" spans="6:20" x14ac:dyDescent="0.2">
@@ -7851,43 +7854,43 @@
       </c>
       <c r="I25">
         <f t="shared" si="3"/>
-        <v>2.7530462309701269</v>
+        <v>4.0271793906958884</v>
       </c>
       <c r="J25">
         <f t="shared" si="4"/>
-        <v>170.90489050244227</v>
+        <v>223.50845618362149</v>
       </c>
       <c r="K25">
         <f t="shared" si="0"/>
-        <v>5.6311462513678654</v>
+        <v>6.9052794110936269</v>
       </c>
       <c r="L25">
         <f t="shared" si="1"/>
-        <v>-0.12505378942761158</v>
+        <v>1.1490793702981499</v>
       </c>
       <c r="M25">
         <f t="shared" si="5"/>
-        <v>310.19829078801064</v>
+        <v>362.80185646918977</v>
       </c>
       <c r="N25">
         <f t="shared" si="6"/>
-        <v>31.611490216873936</v>
+        <v>84.215055898053166</v>
       </c>
       <c r="Q25">
         <f t="shared" si="7"/>
-        <v>1.8140751643719077</v>
+        <v>1.8198895078474591</v>
       </c>
       <c r="R25">
         <f t="shared" si="8"/>
-        <v>87.797052301206719</v>
+        <v>88.078453109864427</v>
       </c>
       <c r="S25">
         <f t="shared" si="9"/>
-        <v>58.239850135170286</v>
+        <v>79.434555195799533</v>
       </c>
       <c r="T25">
         <f t="shared" si="10"/>
-        <v>61.840908118999479</v>
+        <v>77.562269047991066</v>
       </c>
     </row>
     <row r="26" spans="6:20" x14ac:dyDescent="0.2">
@@ -7904,43 +7907,43 @@
       </c>
       <c r="I26">
         <f t="shared" si="3"/>
-        <v>1.4716709702941646</v>
+        <v>2.7458041300199261</v>
       </c>
       <c r="J26">
         <f t="shared" si="4"/>
-        <v>172.37656147273643</v>
+        <v>226.25426031364142</v>
       </c>
       <c r="K26">
         <f t="shared" si="0"/>
-        <v>3.3497709906919031</v>
+        <v>4.6239041504176646</v>
       </c>
       <c r="L26">
         <f t="shared" si="1"/>
-        <v>-0.40642905010357389</v>
+        <v>0.86770410962218758</v>
       </c>
       <c r="M26">
         <f t="shared" si="5"/>
-        <v>313.54806177870256</v>
+        <v>367.42576061960744</v>
       </c>
       <c r="N26">
         <f t="shared" si="6"/>
-        <v>31.205061166770363</v>
+        <v>85.082760007675347</v>
       </c>
       <c r="Q26">
         <f t="shared" si="7"/>
-        <v>1.1837721340688776</v>
+        <v>1.1875662755242267</v>
       </c>
       <c r="R26">
         <f t="shared" si="8"/>
-        <v>88.980824435275593</v>
+        <v>89.26601938538866</v>
       </c>
       <c r="S26">
         <f t="shared" si="9"/>
-        <v>58.254104443616917</v>
+        <v>79.45377023779568</v>
       </c>
       <c r="T26">
         <f t="shared" si="10"/>
-        <v>62.64216906091108</v>
+        <v>79.062145970328729</v>
       </c>
     </row>
     <row r="27" spans="6:20" x14ac:dyDescent="0.2">
@@ -7957,43 +7960,43 @@
       </c>
       <c r="I27">
         <f t="shared" si="3"/>
-        <v>0.1902957096182023</v>
+        <v>1.4644288693439638</v>
       </c>
       <c r="J27">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.7186891829854</v>
       </c>
       <c r="K27">
         <f t="shared" si="0"/>
-        <v>1.0683957300159408</v>
+        <v>2.3425288897417023</v>
       </c>
       <c r="L27">
         <f t="shared" si="1"/>
-        <v>-0.68780431077953619</v>
+        <v>0.58632884894622528</v>
       </c>
       <c r="M27">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.76828950934913</v>
       </c>
       <c r="N27">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.66908885662157</v>
       </c>
       <c r="Q27">
         <f t="shared" si="7"/>
-        <v>0.55346910376584724</v>
+        <v>0.55524304320099427</v>
       </c>
       <c r="R27">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S27">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456265881042398</v>
       </c>
       <c r="T27">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.862142077672246</v>
       </c>
     </row>
     <row r="28" spans="6:20" x14ac:dyDescent="0.2">
@@ -8010,27 +8013,27 @@
       </c>
       <c r="I28">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.18305360866800147</v>
       </c>
       <c r="J28">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.18305360866800147</v>
       </c>
       <c r="L28">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.18305360866800147</v>
       </c>
       <c r="M28">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N28">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q28">
         <f t="shared" si="7"/>
@@ -8038,15 +8041,15 @@
       </c>
       <c r="R28">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S28">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T28">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
     <row r="29" spans="6:20" x14ac:dyDescent="0.2">
@@ -8067,7 +8070,7 @@
       </c>
       <c r="J29">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K29">
         <f t="shared" si="0"/>
@@ -8079,11 +8082,11 @@
       </c>
       <c r="M29">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N29">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q29">
         <f t="shared" si="7"/>
@@ -8091,15 +8094,15 @@
       </c>
       <c r="R29">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S29">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T29">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
     <row r="30" spans="6:20" x14ac:dyDescent="0.2">
@@ -8120,7 +8123,7 @@
       </c>
       <c r="J30">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K30">
         <f t="shared" si="0"/>
@@ -8132,11 +8135,11 @@
       </c>
       <c r="M30">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N30">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q30">
         <f t="shared" si="7"/>
@@ -8144,15 +8147,15 @@
       </c>
       <c r="R30">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S30">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T30">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
     <row r="31" spans="6:20" x14ac:dyDescent="0.2">
@@ -8173,7 +8176,7 @@
       </c>
       <c r="J31">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K31">
         <f t="shared" si="0"/>
@@ -8185,11 +8188,11 @@
       </c>
       <c r="M31">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N31">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q31">
         <f t="shared" si="7"/>
@@ -8197,15 +8200,15 @@
       </c>
       <c r="R31">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S31">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T31">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
     <row r="32" spans="6:20" x14ac:dyDescent="0.2">
@@ -8226,7 +8229,7 @@
       </c>
       <c r="J32">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K32">
         <f t="shared" si="0"/>
@@ -8238,11 +8241,11 @@
       </c>
       <c r="M32">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N32">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q32">
         <f t="shared" si="7"/>
@@ -8250,18 +8253,18 @@
       </c>
       <c r="R32">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S32">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T32">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="33" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:20" x14ac:dyDescent="0.2">
       <c r="F33">
         <v>750</v>
       </c>
@@ -8279,7 +8282,7 @@
       </c>
       <c r="J33">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K33">
         <f t="shared" si="0"/>
@@ -8291,11 +8294,11 @@
       </c>
       <c r="M33">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N33">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q33">
         <f t="shared" si="7"/>
@@ -8303,18 +8306,18 @@
       </c>
       <c r="R33">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S33">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T33">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="34" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:20" x14ac:dyDescent="0.2">
       <c r="F34">
         <v>775</v>
       </c>
@@ -8332,7 +8335,7 @@
       </c>
       <c r="J34">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K34">
         <f t="shared" si="0"/>
@@ -8344,11 +8347,11 @@
       </c>
       <c r="M34">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N34">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q34">
         <f t="shared" si="7"/>
@@ -8356,18 +8359,18 @@
       </c>
       <c r="R34">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S34">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T34">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="35" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:20" x14ac:dyDescent="0.2">
       <c r="F35">
         <v>800</v>
       </c>
@@ -8385,7 +8388,7 @@
       </c>
       <c r="J35">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K35">
         <f t="shared" si="0"/>
@@ -8397,11 +8400,11 @@
       </c>
       <c r="M35">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N35">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q35">
         <f t="shared" si="7"/>
@@ -8409,18 +8412,18 @@
       </c>
       <c r="R35">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S35">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T35">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="36" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:20" x14ac:dyDescent="0.2">
       <c r="F36">
         <v>825</v>
       </c>
@@ -8438,7 +8441,7 @@
       </c>
       <c r="J36">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K36">
         <f t="shared" si="0"/>
@@ -8450,11 +8453,11 @@
       </c>
       <c r="M36">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N36">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q36">
         <f t="shared" si="7"/>
@@ -8462,18 +8465,18 @@
       </c>
       <c r="R36">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S36">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T36">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="37" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:20" x14ac:dyDescent="0.2">
       <c r="F37">
         <v>850</v>
       </c>
@@ -8491,7 +8494,7 @@
       </c>
       <c r="J37">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K37">
         <f t="shared" si="0"/>
@@ -8503,11 +8506,11 @@
       </c>
       <c r="M37">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N37">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q37">
         <f t="shared" si="7"/>
@@ -8515,18 +8518,18 @@
       </c>
       <c r="R37">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S37">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T37">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="38" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:20" x14ac:dyDescent="0.2">
       <c r="F38">
         <v>875</v>
       </c>
@@ -8544,7 +8547,7 @@
       </c>
       <c r="J38">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K38">
         <f t="shared" si="0"/>
@@ -8556,11 +8559,11 @@
       </c>
       <c r="M38">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N38">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q38">
         <f t="shared" si="7"/>
@@ -8568,18 +8571,18 @@
       </c>
       <c r="R38">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S38">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T38">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="39" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:20" x14ac:dyDescent="0.2">
       <c r="F39">
         <v>900</v>
       </c>
@@ -8597,7 +8600,7 @@
       </c>
       <c r="J39">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K39">
         <f t="shared" si="0"/>
@@ -8609,11 +8612,11 @@
       </c>
       <c r="M39">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N39">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q39">
         <f t="shared" si="7"/>
@@ -8621,18 +8624,18 @@
       </c>
       <c r="R39">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S39">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T39">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="40" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:20" x14ac:dyDescent="0.2">
       <c r="F40">
         <v>925</v>
       </c>
@@ -8650,7 +8653,7 @@
       </c>
       <c r="J40">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K40">
         <f t="shared" si="0"/>
@@ -8662,11 +8665,11 @@
       </c>
       <c r="M40">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N40">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q40">
         <f t="shared" si="7"/>
@@ -8674,18 +8677,18 @@
       </c>
       <c r="R40">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S40">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T40">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="41" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:20" x14ac:dyDescent="0.2">
       <c r="F41">
         <v>950</v>
       </c>
@@ -8703,7 +8706,7 @@
       </c>
       <c r="J41">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K41">
         <f t="shared" si="0"/>
@@ -8715,11 +8718,11 @@
       </c>
       <c r="M41">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N41">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q41">
         <f t="shared" si="7"/>
@@ -8727,18 +8730,18 @@
       </c>
       <c r="R41">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S41">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T41">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="42" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:20" x14ac:dyDescent="0.2">
       <c r="F42">
         <v>975</v>
       </c>
@@ -8756,7 +8759,7 @@
       </c>
       <c r="J42">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K42">
         <f t="shared" si="0"/>
@@ -8768,11 +8771,11 @@
       </c>
       <c r="M42">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N42">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q42">
         <f t="shared" si="7"/>
@@ -8780,18 +8783,18 @@
       </c>
       <c r="R42">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S42">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T42">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="43" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:20" x14ac:dyDescent="0.2">
       <c r="F43">
         <v>1000</v>
       </c>
@@ -8809,7 +8812,7 @@
       </c>
       <c r="J43">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K43">
         <f t="shared" si="0"/>
@@ -8821,11 +8824,11 @@
       </c>
       <c r="M43">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N43">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q43">
         <f t="shared" si="7"/>
@@ -8833,18 +8836,18 @@
       </c>
       <c r="R43">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S43">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T43">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="44" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:20" x14ac:dyDescent="0.2">
       <c r="F44">
         <v>1025</v>
       </c>
@@ -8862,7 +8865,7 @@
       </c>
       <c r="J44">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K44">
         <f t="shared" si="0"/>
@@ -8874,11 +8877,11 @@
       </c>
       <c r="M44">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N44">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q44">
         <f t="shared" si="7"/>
@@ -8886,18 +8889,18 @@
       </c>
       <c r="R44">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S44">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T44">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="45" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:20" x14ac:dyDescent="0.2">
       <c r="F45">
         <v>1050</v>
       </c>
@@ -8915,7 +8918,7 @@
       </c>
       <c r="J45">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K45">
         <f t="shared" si="0"/>
@@ -8927,11 +8930,11 @@
       </c>
       <c r="M45">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N45">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q45">
         <f t="shared" si="7"/>
@@ -8939,18 +8942,18 @@
       </c>
       <c r="R45">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S45">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T45">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="46" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:20" x14ac:dyDescent="0.2">
       <c r="F46">
         <v>1075</v>
       </c>
@@ -8968,7 +8971,7 @@
       </c>
       <c r="J46">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K46">
         <f t="shared" si="0"/>
@@ -8980,11 +8983,11 @@
       </c>
       <c r="M46">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N46">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q46">
         <f t="shared" si="7"/>
@@ -8992,18 +8995,21 @@
       </c>
       <c r="R46">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S46">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T46">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="47" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="C47" s="18">
+        <v>42717</v>
+      </c>
       <c r="F47">
         <v>1100</v>
       </c>
@@ -9021,7 +9027,7 @@
       </c>
       <c r="J47">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K47">
         <f t="shared" si="0"/>
@@ -9033,11 +9039,11 @@
       </c>
       <c r="M47">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N47">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q47">
         <f t="shared" si="7"/>
@@ -9045,18 +9051,18 @@
       </c>
       <c r="R47">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S47">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T47">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="48" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:20" x14ac:dyDescent="0.2">
       <c r="F48">
         <v>1125</v>
       </c>
@@ -9074,7 +9080,7 @@
       </c>
       <c r="J48">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K48">
         <f t="shared" si="0"/>
@@ -9086,11 +9092,11 @@
       </c>
       <c r="M48">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N48">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q48">
         <f t="shared" si="7"/>
@@ -9098,18 +9104,18 @@
       </c>
       <c r="R48">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S48">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T48">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="49" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:20" x14ac:dyDescent="0.2">
       <c r="F49">
         <v>1150</v>
       </c>
@@ -9127,7 +9133,7 @@
       </c>
       <c r="J49">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K49">
         <f t="shared" si="0"/>
@@ -9139,11 +9145,11 @@
       </c>
       <c r="M49">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N49">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q49">
         <f t="shared" si="7"/>
@@ -9151,18 +9157,18 @@
       </c>
       <c r="R49">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S49">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T49">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="50" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:20" x14ac:dyDescent="0.2">
       <c r="F50">
         <v>1175</v>
       </c>
@@ -9180,7 +9186,7 @@
       </c>
       <c r="J50">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K50">
         <f t="shared" si="0"/>
@@ -9192,11 +9198,11 @@
       </c>
       <c r="M50">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N50">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q50">
         <f t="shared" si="7"/>
@@ -9204,18 +9210,18 @@
       </c>
       <c r="R50">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S50">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T50">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="51" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:20" x14ac:dyDescent="0.2">
       <c r="F51">
         <v>1200</v>
       </c>
@@ -9233,7 +9239,7 @@
       </c>
       <c r="J51">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K51">
         <f t="shared" si="0"/>
@@ -9245,11 +9251,11 @@
       </c>
       <c r="M51">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N51">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q51">
         <f t="shared" si="7"/>
@@ -9257,18 +9263,18 @@
       </c>
       <c r="R51">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S51">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T51">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="52" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:20" x14ac:dyDescent="0.2">
       <c r="F52">
         <v>1225</v>
       </c>
@@ -9286,7 +9292,7 @@
       </c>
       <c r="J52">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K52">
         <f t="shared" si="0"/>
@@ -9298,11 +9304,11 @@
       </c>
       <c r="M52">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N52">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q52">
         <f t="shared" si="7"/>
@@ -9310,18 +9316,18 @@
       </c>
       <c r="R52">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S52">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T52">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="53" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:20" x14ac:dyDescent="0.2">
       <c r="F53">
         <v>1250</v>
       </c>
@@ -9339,7 +9345,7 @@
       </c>
       <c r="J53">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K53">
         <f t="shared" si="0"/>
@@ -9351,11 +9357,11 @@
       </c>
       <c r="M53">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N53">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q53">
         <f t="shared" si="7"/>
@@ -9363,18 +9369,18 @@
       </c>
       <c r="R53">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S53">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T53">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="54" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:20" x14ac:dyDescent="0.2">
       <c r="F54">
         <v>1275</v>
       </c>
@@ -9392,7 +9398,7 @@
       </c>
       <c r="J54">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K54">
         <f t="shared" si="0"/>
@@ -9404,11 +9410,11 @@
       </c>
       <c r="M54">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N54">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q54">
         <f t="shared" si="7"/>
@@ -9416,18 +9422,18 @@
       </c>
       <c r="R54">
         <f>Q54+R53</f>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S54">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T54">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="55" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:20" x14ac:dyDescent="0.2">
       <c r="F55">
         <v>1300</v>
       </c>
@@ -9445,7 +9451,7 @@
       </c>
       <c r="J55">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K55">
         <f t="shared" si="0"/>
@@ -9457,11 +9463,11 @@
       </c>
       <c r="M55">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N55">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q55">
         <f t="shared" si="7"/>
@@ -9469,18 +9475,22 @@
       </c>
       <c r="R55">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S55">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T55">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="56" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="C56">
+        <f>13/12</f>
+        <v>1.0833333333333333</v>
+      </c>
       <c r="F56">
         <v>1325</v>
       </c>
@@ -9498,7 +9508,7 @@
       </c>
       <c r="J56">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K56">
         <f t="shared" si="0"/>
@@ -9510,11 +9520,11 @@
       </c>
       <c r="M56">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N56">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q56">
         <f t="shared" si="7"/>
@@ -9522,18 +9532,22 @@
       </c>
       <c r="R56">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S56">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T56">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="57" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="C57">
+        <f>530/2/180 * 2*PI()*C15 /120</f>
+        <v>1.2063861233889139</v>
+      </c>
       <c r="F57">
         <v>1350</v>
       </c>
@@ -9551,7 +9565,7 @@
       </c>
       <c r="J57">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K57">
         <f t="shared" si="0"/>
@@ -9563,11 +9577,11 @@
       </c>
       <c r="M57">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N57">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q57">
         <f t="shared" si="7"/>
@@ -9575,18 +9589,18 @@
       </c>
       <c r="R57">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S57">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T57">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="58" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:20" x14ac:dyDescent="0.2">
       <c r="F58">
         <v>1375</v>
       </c>
@@ -9604,7 +9618,7 @@
       </c>
       <c r="J58">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K58">
         <f t="shared" si="0"/>
@@ -9616,11 +9630,11 @@
       </c>
       <c r="M58">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N58">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q58">
         <f t="shared" si="7"/>
@@ -9628,18 +9642,22 @@
       </c>
       <c r="R58">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S58">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T58">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="59" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="C59">
+        <f>130/(2*PI()*C15) * 180</f>
+        <v>237.96969126839303</v>
+      </c>
       <c r="F59">
         <v>1400</v>
       </c>
@@ -9657,7 +9675,7 @@
       </c>
       <c r="J59">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K59">
         <f t="shared" si="0"/>
@@ -9669,11 +9687,11 @@
       </c>
       <c r="M59">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N59">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q59">
         <f t="shared" si="7"/>
@@ -9681,18 +9699,22 @@
       </c>
       <c r="R59">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S59">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T59">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="60" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:20" x14ac:dyDescent="0.2">
+      <c r="C60">
+        <f>28000/(2*PI()*15.65)</f>
+        <v>284.75005792799163</v>
+      </c>
       <c r="F60">
         <v>1425</v>
       </c>
@@ -9710,7 +9732,7 @@
       </c>
       <c r="J60">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K60">
         <f t="shared" si="0"/>
@@ -9722,11 +9744,11 @@
       </c>
       <c r="M60">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N60">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q60">
         <f t="shared" si="7"/>
@@ -9734,18 +9756,18 @@
       </c>
       <c r="R60">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S60">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T60">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="61" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:20" x14ac:dyDescent="0.2">
       <c r="F61">
         <v>1450</v>
       </c>
@@ -9763,7 +9785,7 @@
       </c>
       <c r="J61">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K61">
         <f t="shared" si="0"/>
@@ -9775,11 +9797,11 @@
       </c>
       <c r="M61">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N61">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q61">
         <f t="shared" si="7"/>
@@ -9787,18 +9809,18 @@
       </c>
       <c r="R61">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S61">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T61">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="62" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:20" x14ac:dyDescent="0.2">
       <c r="F62">
         <v>1475</v>
       </c>
@@ -9816,7 +9838,7 @@
       </c>
       <c r="J62">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K62">
         <f t="shared" si="0"/>
@@ -9828,11 +9850,11 @@
       </c>
       <c r="M62">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N62">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q62">
         <f t="shared" si="7"/>
@@ -9840,18 +9862,18 @@
       </c>
       <c r="R62">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S62">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T62">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="63" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:20" x14ac:dyDescent="0.2">
       <c r="F63">
         <v>1500</v>
       </c>
@@ -9869,7 +9891,7 @@
       </c>
       <c r="J63">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K63">
         <f t="shared" si="0"/>
@@ -9881,11 +9903,11 @@
       </c>
       <c r="M63">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N63">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q63">
         <f t="shared" si="7"/>
@@ -9893,18 +9915,18 @@
       </c>
       <c r="R63">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S63">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T63">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
-    <row r="64" spans="6:20" x14ac:dyDescent="0.2">
+    <row r="64" spans="3:20" x14ac:dyDescent="0.2">
       <c r="F64">
         <v>1525</v>
       </c>
@@ -9922,7 +9944,7 @@
       </c>
       <c r="J64">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K64">
         <f t="shared" si="0"/>
@@ -9934,11 +9956,11 @@
       </c>
       <c r="M64">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N64">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q64">
         <f t="shared" si="7"/>
@@ -9946,15 +9968,15 @@
       </c>
       <c r="R64">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S64">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T64">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
     <row r="65" spans="6:20" x14ac:dyDescent="0.2">
@@ -9975,7 +9997,7 @@
       </c>
       <c r="J65">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K65">
         <f t="shared" si="0"/>
@@ -9987,11 +10009,11 @@
       </c>
       <c r="M65">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N65">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q65">
         <f t="shared" si="7"/>
@@ -9999,15 +10021,15 @@
       </c>
       <c r="R65">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S65">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T65">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
     <row r="66" spans="6:20" x14ac:dyDescent="0.2">
@@ -10028,7 +10050,7 @@
       </c>
       <c r="J66">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K66">
         <f t="shared" si="0"/>
@@ -10040,11 +10062,11 @@
       </c>
       <c r="M66">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N66">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q66">
         <f t="shared" si="7"/>
@@ -10052,15 +10074,15 @@
       </c>
       <c r="R66">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S66">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T66">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
     <row r="67" spans="6:20" x14ac:dyDescent="0.2">
@@ -10081,7 +10103,7 @@
       </c>
       <c r="J67">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K67">
         <f t="shared" si="0"/>
@@ -10093,11 +10115,11 @@
       </c>
       <c r="M67">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N67">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q67">
         <f t="shared" si="7"/>
@@ -10105,15 +10127,15 @@
       </c>
       <c r="R67">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S67">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T67">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
     <row r="68" spans="6:20" x14ac:dyDescent="0.2">
@@ -10134,7 +10156,7 @@
       </c>
       <c r="J68">
         <f t="shared" si="4"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K68">
         <f t="shared" ref="K68:K74" si="11">I68+G68</f>
@@ -10146,11 +10168,11 @@
       </c>
       <c r="M68">
         <f t="shared" si="5"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N68">
         <f t="shared" si="6"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q68">
         <f t="shared" si="7"/>
@@ -10158,15 +10180,15 @@
       </c>
       <c r="R68">
         <f t="shared" si="8"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S68">
         <f t="shared" si="9"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T68">
         <f t="shared" si="10"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
     <row r="69" spans="6:20" x14ac:dyDescent="0.2">
@@ -10187,7 +10209,7 @@
       </c>
       <c r="J69">
         <f t="shared" ref="J69:J74" si="15">I69+J68</f>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K69">
         <f t="shared" si="11"/>
@@ -10199,11 +10221,11 @@
       </c>
       <c r="M69">
         <f t="shared" ref="M69:M74" si="16">K69+M68</f>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N69">
         <f t="shared" ref="N69:N74" si="17">L69+N68</f>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q69">
         <f t="shared" ref="Q69:Q74" si="18">360/(2*PI())*$P$3*(K69-L69)/$C$14</f>
@@ -10211,15 +10233,15 @@
       </c>
       <c r="R69">
         <f t="shared" ref="R69:R74" si="19">Q69+R68</f>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S69">
         <f t="shared" ref="S69:S74" si="20">S68+$P$3*((L69+K69)/2*COS(RADIANS(R69)))</f>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T69">
         <f t="shared" ref="T69:T74" si="21">T68+$P$3*((L69+K69)/2*SIN(RADIANS(R69)))</f>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
     <row r="70" spans="6:20" x14ac:dyDescent="0.2">
@@ -10240,7 +10262,7 @@
       </c>
       <c r="J70">
         <f t="shared" si="15"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K70">
         <f t="shared" si="11"/>
@@ -10252,11 +10274,11 @@
       </c>
       <c r="M70">
         <f t="shared" si="16"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N70">
         <f t="shared" si="17"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q70">
         <f t="shared" si="18"/>
@@ -10264,15 +10286,15 @@
       </c>
       <c r="R70">
         <f t="shared" si="19"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S70">
         <f t="shared" si="20"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T70">
         <f t="shared" si="21"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
     <row r="71" spans="6:20" x14ac:dyDescent="0.2">
@@ -10293,7 +10315,7 @@
       </c>
       <c r="J71">
         <f t="shared" si="15"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K71">
         <f t="shared" si="11"/>
@@ -10305,11 +10327,11 @@
       </c>
       <c r="M71">
         <f t="shared" si="16"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N71">
         <f t="shared" si="17"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q71">
         <f t="shared" si="18"/>
@@ -10317,15 +10339,15 @@
       </c>
       <c r="R71">
         <f t="shared" si="19"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S71">
         <f t="shared" si="20"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T71">
         <f t="shared" si="21"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
     <row r="72" spans="6:20" x14ac:dyDescent="0.2">
@@ -10346,7 +10368,7 @@
       </c>
       <c r="J72">
         <f t="shared" si="15"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K72">
         <f t="shared" si="11"/>
@@ -10358,11 +10380,11 @@
       </c>
       <c r="M72">
         <f t="shared" si="16"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N72">
         <f t="shared" si="17"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q72">
         <f t="shared" si="18"/>
@@ -10370,15 +10392,15 @@
       </c>
       <c r="R72">
         <f t="shared" si="19"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S72">
         <f t="shared" si="20"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T72">
         <f t="shared" si="21"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
     <row r="73" spans="6:20" x14ac:dyDescent="0.2">
@@ -10399,7 +10421,7 @@
       </c>
       <c r="J73">
         <f t="shared" si="15"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K73">
         <f t="shared" si="11"/>
@@ -10411,11 +10433,11 @@
       </c>
       <c r="M73">
         <f t="shared" si="16"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N73">
         <f t="shared" si="17"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q73">
         <f t="shared" si="18"/>
@@ -10423,15 +10445,15 @@
       </c>
       <c r="R73">
         <f t="shared" si="19"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S73">
         <f t="shared" si="20"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T73">
         <f t="shared" si="21"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
     <row r="74" spans="6:20" x14ac:dyDescent="0.2">
@@ -10452,7 +10474,7 @@
       </c>
       <c r="J74">
         <f t="shared" si="15"/>
-        <v>172.56685718235462</v>
+        <v>227.90174279165339</v>
       </c>
       <c r="K74">
         <f t="shared" si="11"/>
@@ -10464,11 +10486,11 @@
       </c>
       <c r="M74">
         <f t="shared" si="16"/>
-        <v>314.6164575087185</v>
+        <v>369.95134311801712</v>
       </c>
       <c r="N74">
         <f t="shared" si="17"/>
-        <v>30.517256855990826</v>
+        <v>85.852142465289575</v>
       </c>
       <c r="Q74">
         <f t="shared" si="18"/>
@@ -10476,15 +10498,15 @@
       </c>
       <c r="R74">
         <f t="shared" si="19"/>
-        <v>89.534293539041443</v>
+        <v>89.821262428589648</v>
       </c>
       <c r="S74">
         <f t="shared" si="20"/>
-        <v>58.254946702901613</v>
+        <v>79.456577836448233</v>
       </c>
       <c r="T74">
         <f t="shared" si="21"/>
-        <v>62.745789782483726</v>
+        <v>79.962141591090187</v>
       </c>
     </row>
     <row r="85" spans="3:4" x14ac:dyDescent="0.2">
@@ -10493,7 +10515,7 @@
       </c>
       <c r="D85">
         <f>PI()/2*C14/P3</f>
-        <v>285.57692307692309</v>
+        <v>284.66453674121408</v>
       </c>
     </row>
     <row r="86" spans="3:4" x14ac:dyDescent="0.2">

</xml_diff>